<commit_message>
Added table of T6SS markers
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/projects/salmonella/work/20250712/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E384F3-434D-9F4F-831A-AB9896F5342A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3BE423-8C6E-B54B-9917-89A2FD5C7429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="134">
   <si>
     <t>Accession</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>aravind</t>
-  </si>
-  <si>
-    <t>HslUClpX-AAA</t>
   </si>
   <si>
     <t>PF09937</t>
@@ -824,11 +821,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E649C-559B-754A-9F35-CCF19D3C1FE3}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +866,7 @@
         <v>88</v>
       </c>
       <c r="D2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3"/>
       <c r="J2" s="3"/>
@@ -887,7 +884,7 @@
         <v>99</v>
       </c>
       <c r="D3" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="3"/>
       <c r="J3" s="3"/>
@@ -905,7 +902,7 @@
         <v>99</v>
       </c>
       <c r="D4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3"/>
       <c r="J4" s="3"/>
@@ -1053,7 +1050,7 @@
         <v>87</v>
       </c>
       <c r="D14" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1067,7 +1064,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1151,7 +1148,7 @@
         <v>88</v>
       </c>
       <c r="D21" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1165,7 +1162,7 @@
         <v>99</v>
       </c>
       <c r="D22" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1323,7 +1320,7 @@
         <v>87</v>
       </c>
       <c r="D33" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1337,7 +1334,7 @@
         <v>87</v>
       </c>
       <c r="D34" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1541,27 +1538,13 @@
         <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D49" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1653,7 +1636,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>69</v>
@@ -1661,7 +1644,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>124</v>
@@ -1669,7 +1652,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>70</v>
@@ -1680,13 +1663,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
         <v>132</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added script to classify genomic sites based on gene composition
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/projects/salmonella/work/20250712/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\_home_leep_rfsouza\git\10ksgt6ss\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3BE423-8C6E-B54B-9917-89A2FD5C7429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A86111-2212-4EF8-8E42-6D6A820A9AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="4" r:id="rId1"/>
     <sheet name="pfam" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="210">
   <si>
     <t>Accession</t>
   </si>
@@ -306,9 +307,6 @@
     <t>ClpV</t>
   </si>
   <si>
-    <t>VipA</t>
-  </si>
-  <si>
     <t>TssE</t>
   </si>
   <si>
@@ -436,13 +434,244 @@
   </si>
   <si>
     <t>PF13886</t>
+  </si>
+  <si>
+    <t>TssB</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>orderby</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>detects</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>Effectors</t>
+  </si>
+  <si>
+    <t>T6SS</t>
+  </si>
+  <si>
+    <t>VgrG-like</t>
+  </si>
+  <si>
+    <t>HMMs w/ hits in T6SS, phage and/or tailocins</t>
+  </si>
+  <si>
+    <t>Base complex</t>
+  </si>
+  <si>
+    <t>Sheath</t>
+  </si>
+  <si>
+    <t>TssH</t>
+  </si>
+  <si>
+    <t>ATPase</t>
+  </si>
+  <si>
+    <t>Membrane complex</t>
+  </si>
+  <si>
+    <t>Adaptors</t>
+  </si>
+  <si>
+    <t>MIX</t>
+  </si>
+  <si>
+    <t>Phage</t>
+  </si>
+  <si>
+    <t>GPW_gp25</t>
+  </si>
+  <si>
+    <t>Phage_GPD</t>
+  </si>
+  <si>
+    <t>Phage_spike</t>
+  </si>
+  <si>
+    <t>Phage tail components</t>
+  </si>
+  <si>
+    <t>Phage_T4_gp19</t>
+  </si>
+  <si>
+    <t>HCP-like</t>
+  </si>
+  <si>
+    <t>Phage_tube</t>
+  </si>
+  <si>
+    <t>Mu-like_gpT</t>
+  </si>
+  <si>
+    <t>Phage_sheath_1</t>
+  </si>
+  <si>
+    <t>VipA/B-like</t>
+  </si>
+  <si>
+    <t>Phage_sheath_1C</t>
+  </si>
+  <si>
+    <t>Phage_tail_S</t>
+  </si>
+  <si>
+    <t>Baseplate-like</t>
+  </si>
+  <si>
+    <t>Phage_tail_X</t>
+  </si>
+  <si>
+    <t>Phage_pRha</t>
+  </si>
+  <si>
+    <t>Phage fiber</t>
+  </si>
+  <si>
+    <t>gp37_C</t>
+  </si>
+  <si>
+    <t>gpW</t>
+  </si>
+  <si>
+    <t>Phage_fiber</t>
+  </si>
+  <si>
+    <t>Phage_fiber_2</t>
+  </si>
+  <si>
+    <t>P2_Phage_GpR</t>
+  </si>
+  <si>
+    <t>Other tail components</t>
+  </si>
+  <si>
+    <t>PhageMin_Tail</t>
+  </si>
+  <si>
+    <t>Phage_ASH</t>
+  </si>
+  <si>
+    <t>Phage_CP76</t>
+  </si>
+  <si>
+    <t>Phage_GPL</t>
+  </si>
+  <si>
+    <t>Phage_P2_GpU</t>
+  </si>
+  <si>
+    <t>Phage_T4_gp36</t>
+  </si>
+  <si>
+    <t>Phage_GPO</t>
+  </si>
+  <si>
+    <t>Phage_P2_GpE</t>
+  </si>
+  <si>
+    <t>Phage_TAC_10</t>
+  </si>
+  <si>
+    <t>Phage_TAC_7</t>
+  </si>
+  <si>
+    <t>Phage_AlpA</t>
+  </si>
+  <si>
+    <t>Other phage components</t>
+  </si>
+  <si>
+    <t>Phage-MuB_C</t>
+  </si>
+  <si>
+    <t>Phage_Cox</t>
+  </si>
+  <si>
+    <t>Phage_CI_C</t>
+  </si>
+  <si>
+    <t>Phage_CI_repr</t>
+  </si>
+  <si>
+    <t>Phage_holin_2_3</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_1</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_2</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_6</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_1</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_2</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_3</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_4</t>
+  </si>
+  <si>
+    <t>Phage_integrase</t>
+  </si>
+  <si>
+    <t>Phage_lysis</t>
+  </si>
+  <si>
+    <t>Phage_lysozyme</t>
+  </si>
+  <si>
+    <t>Phage_term_smal</t>
+  </si>
+  <si>
+    <t>Phage_attach</t>
+  </si>
+  <si>
+    <t>Phage_cap_E</t>
+  </si>
+  <si>
+    <t>Phage_gp49_66</t>
+  </si>
+  <si>
+    <t>Phage_GPA</t>
+  </si>
+  <si>
+    <t>Phage_cap_P2</t>
+  </si>
+  <si>
+    <t>Phage_portal</t>
+  </si>
+  <si>
+    <t>Phage_portal_2</t>
+  </si>
+  <si>
+    <t>Phage_connector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,6 +702,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -495,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -506,6 +754,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -821,43 +1079,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E649C-559B-754A-9F35-CCF19D3C1FE3}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>125</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F1" s="3"/>
       <c r="H1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -868,180 +1126,180 @@
       <c r="D2" s="7">
         <v>0</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="H2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="7">
         <v>0</v>
       </c>
+      <c r="F3" s="3"/>
       <c r="H3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
       </c>
+      <c r="F4" s="3"/>
       <c r="H4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
+      <c r="F5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1053,9 +1311,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>37</v>
@@ -1067,54 +1325,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>89</v>
@@ -1123,12 +1381,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
         <v>89</v>
@@ -1137,12 +1395,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
         <v>88</v>
@@ -1151,170 +1409,170 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="7">
         <v>1</v>
       </c>
+      <c r="F26" s="3"/>
       <c r="H26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D32" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
         <v>87</v>
@@ -1323,12 +1581,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
         <v>87</v>
@@ -1337,51 +1595,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="D35" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
       </c>
       <c r="D37" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>86</v>
@@ -1393,9 +1651,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
         <v>69</v>
@@ -1407,23 +1665,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>31</v>
@@ -1435,9 +1693,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>52</v>
@@ -1449,9 +1707,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>74</v>
@@ -1463,9 +1721,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>55</v>
@@ -1477,9 +1735,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>58</v>
@@ -1491,9 +1749,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>61</v>
@@ -1505,9 +1763,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>34</v>
@@ -1519,9 +1777,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>49</v>
@@ -1533,9 +1791,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
         <v>87</v>
@@ -1544,6 +1802,20 @@
         <v>87</v>
       </c>
       <c r="D49" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1573,6 +1845,7 @@
     <hyperlink ref="C46" r:id="rId16" display="https://pfam.xfam.org/family/PF17643" xr:uid="{7253D2E3-E26C-B247-AB7C-53C75C0B5CE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -1581,18 +1854,18 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="171" workbookViewId="0">
-      <selection sqref="A1:D30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1882,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1623,7 +1896,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1634,25 +1907,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>130</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>70</v>
@@ -1661,18 +1934,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
         <v>131</v>
       </c>
-      <c r="C7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1683,7 +1956,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
@@ -1694,7 +1967,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
@@ -1705,7 +1978,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1716,7 +1989,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1727,7 +2000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1738,7 +2011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1749,7 +2022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1763,7 +2036,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1777,7 +2050,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1791,7 +2064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1802,7 +2075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1813,7 +2086,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1827,7 +2100,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1838,7 +2111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1852,7 +2125,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -1863,7 +2136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1874,7 +2147,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1885,7 +2158,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1896,7 +2169,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1907,7 +2180,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1918,7 +2191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1929,7 +2202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1999,4 +2272,1025 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57490B66-446A-4941-B19B-A7B1B51EF347}">
+  <dimension ref="A1:E70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added phage sheet to t6ss.xlsx
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/git/10ksgt6ss/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFBABB1-CC80-C74B-A954-80C88FDECF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3E3DF0-545C-0C48-9256-6F6C53FB2014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="all" sheetId="4" r:id="rId1"/>
-    <sheet name="pfam" sheetId="1" r:id="rId2"/>
+    <sheet name="t6ss" sheetId="4" r:id="rId1"/>
+    <sheet name="phage" sheetId="5" r:id="rId2"/>
+    <sheet name="t6ss description" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="196">
   <si>
     <t>Accession</t>
   </si>
@@ -439,13 +440,196 @@
   </si>
   <si>
     <t>Phage_GPD</t>
+  </si>
+  <si>
+    <t>VgrG-like</t>
+  </si>
+  <si>
+    <t>HMMs w/ hits in T6SS, phage and/or tailocins</t>
+  </si>
+  <si>
+    <t>GPW_gp25</t>
+  </si>
+  <si>
+    <t>Phage_spike</t>
+  </si>
+  <si>
+    <t>Phage tail components</t>
+  </si>
+  <si>
+    <t>Phage_T4_gp19</t>
+  </si>
+  <si>
+    <t>HCP-like</t>
+  </si>
+  <si>
+    <t>Phage_tube</t>
+  </si>
+  <si>
+    <t>Mu-like_gpT</t>
+  </si>
+  <si>
+    <t>Phage_sheath_1</t>
+  </si>
+  <si>
+    <t>VipA/B-like</t>
+  </si>
+  <si>
+    <t>Phage_sheath_1C</t>
+  </si>
+  <si>
+    <t>Phage_tail_S</t>
+  </si>
+  <si>
+    <t>Baseplate-like</t>
+  </si>
+  <si>
+    <t>Phage_tail_X</t>
+  </si>
+  <si>
+    <t>Phage_pRha</t>
+  </si>
+  <si>
+    <t>Phage fiber</t>
+  </si>
+  <si>
+    <t>gp37_C</t>
+  </si>
+  <si>
+    <t>gpW</t>
+  </si>
+  <si>
+    <t>Phage_fiber</t>
+  </si>
+  <si>
+    <t>Phage_fiber_2</t>
+  </si>
+  <si>
+    <t>P2_Phage_GpR</t>
+  </si>
+  <si>
+    <t>Other tail components</t>
+  </si>
+  <si>
+    <t>PhageMin_Tail</t>
+  </si>
+  <si>
+    <t>Phage_ASH</t>
+  </si>
+  <si>
+    <t>Phage_CP76</t>
+  </si>
+  <si>
+    <t>Phage_GPL</t>
+  </si>
+  <si>
+    <t>Phage_P2_GpU</t>
+  </si>
+  <si>
+    <t>Phage_T4_gp36</t>
+  </si>
+  <si>
+    <t>Phage_GPO</t>
+  </si>
+  <si>
+    <t>Phage_P2_GpE</t>
+  </si>
+  <si>
+    <t>Phage_TAC_10</t>
+  </si>
+  <si>
+    <t>Phage_TAC_7</t>
+  </si>
+  <si>
+    <t>Phage_AlpA</t>
+  </si>
+  <si>
+    <t>Other phage components</t>
+  </si>
+  <si>
+    <t>Phage-MuB_C</t>
+  </si>
+  <si>
+    <t>Phage_Cox</t>
+  </si>
+  <si>
+    <t>Phage_CI_C</t>
+  </si>
+  <si>
+    <t>Phage_CI_repr</t>
+  </si>
+  <si>
+    <t>Phage_holin_2_3</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_1</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_2</t>
+  </si>
+  <si>
+    <t>Phage_holin_3_6</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_1</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_2</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_3</t>
+  </si>
+  <si>
+    <t>Phage_int_SAM_4</t>
+  </si>
+  <si>
+    <t>Phage_integrase</t>
+  </si>
+  <si>
+    <t>Phage_lysis</t>
+  </si>
+  <si>
+    <t>Phage_lysozyme</t>
+  </si>
+  <si>
+    <t>Phage_term_smal</t>
+  </si>
+  <si>
+    <t>Phage_attach</t>
+  </si>
+  <si>
+    <t>Phage_cap_E</t>
+  </si>
+  <si>
+    <t>Phage_gp49_66</t>
+  </si>
+  <si>
+    <t>Phage_GPA</t>
+  </si>
+  <si>
+    <t>Phage_cap_P2</t>
+  </si>
+  <si>
+    <t>Phage_portal</t>
+  </si>
+  <si>
+    <t>Phage_portal_2</t>
+  </si>
+  <si>
+    <t>Phage_connector</t>
+  </si>
+  <si>
+    <t>secondrow</t>
+  </si>
+  <si>
+    <t>firstrow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -476,6 +660,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -485,7 +688,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -493,12 +696,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,6 +726,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -826,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E649C-559B-754A-9F35-CCF19D3C1FE3}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1595,6 +1825,715 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90900223-5810-9042-B674-407BA3CF946F}">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61C3554-8D9E-3642-8F25-3AAA47A8A2FB}">
   <dimension ref="A1:G30"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changing zoom in t6ss.xlsx
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/git/10ksgt6ss/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3E3DF0-545C-0C48-9256-6F6C53FB2014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4326C33-2D5A-5C44-A975-02C28E1E61AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="2" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
   <sheets>
     <sheet name="t6ss" sheetId="4" r:id="rId1"/>
@@ -1828,7 +1828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90900223-5810-9042-B674-407BA3CF946F}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2537,7 +2539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61C3554-8D9E-3642-8F25-3AAA47A8A2FB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="171" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding MIX to t6ss.xlsx
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfsouza/git/10ksgt6ss/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4326C33-2D5A-5C44-A975-02C28E1E61AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C28FA-D30B-2B48-A4A8-44F6DDAC7047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="2" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
   <sheets>
     <sheet name="t6ss" sheetId="4" r:id="rId1"/>
     <sheet name="phage" sheetId="5" r:id="rId2"/>
     <sheet name="t6ss description" sheetId="1" r:id="rId3"/>
+    <sheet name="sorting" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="222">
   <si>
     <t>Accession</t>
   </si>
@@ -623,6 +624,84 @@
   </si>
   <si>
     <t>firstrow</t>
+  </si>
+  <si>
+    <t>cdd</t>
+  </si>
+  <si>
+    <t>MIX</t>
+  </si>
+  <si>
+    <t>MIX_I</t>
+  </si>
+  <si>
+    <t>MIX_II</t>
+  </si>
+  <si>
+    <t>MIX_III</t>
+  </si>
+  <si>
+    <t>MIX_IV</t>
+  </si>
+  <si>
+    <t>MIX_V</t>
+  </si>
+  <si>
+    <t>countAs</t>
+  </si>
+  <si>
+    <t>sameAs</t>
+  </si>
+  <si>
+    <t>T6SS</t>
+  </si>
+  <si>
+    <t>Effectors</t>
+  </si>
+  <si>
+    <t>PAAR_1</t>
+  </si>
+  <si>
+    <t>PAAR_2</t>
+  </si>
+  <si>
+    <t>PAAR_3</t>
+  </si>
+  <si>
+    <t>PAAR_4</t>
+  </si>
+  <si>
+    <t>PAAR_5</t>
+  </si>
+  <si>
+    <t>PAAR_CT_1</t>
+  </si>
+  <si>
+    <t>PAAR_CT_2</t>
+  </si>
+  <si>
+    <t>PAAR_like</t>
+  </si>
+  <si>
+    <t>PAAR_RHS</t>
+  </si>
+  <si>
+    <t>Base complex</t>
+  </si>
+  <si>
+    <t>Sheath</t>
+  </si>
+  <si>
+    <t>ATPase</t>
+  </si>
+  <si>
+    <t>Membrane complex</t>
+  </si>
+  <si>
+    <t>Adaptors</t>
+  </si>
+  <si>
+    <t>Phage</t>
   </si>
 </sst>
 </file>
@@ -688,7 +767,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -711,12 +790,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -738,6 +826,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E649C-559B-754A-9F35-CCF19D3C1FE3}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -1071,16 +1167,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F1" s="3"/>
@@ -1791,6 +1887,90 @@
         <v>87</v>
       </c>
       <c r="D50" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" t="s">
+        <v>197</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1828,9 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90900223-5810-9042-B674-407BA3CF946F}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2539,9 +2717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61C3554-8D9E-3642-8F25-3AAA47A8A2FB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView zoomScale="164" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2958,4 +3134,1966 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5E165A-D48E-D143-9ECC-41E4D489F132}">
+  <dimension ref="A1:F106"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" t="s">
+        <v>216</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>216</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" t="s">
+        <v>219</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" t="s">
+        <v>219</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" t="s">
+        <v>205</v>
+      </c>
+      <c r="D51" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" t="s">
+        <v>197</v>
+      </c>
+      <c r="E52" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>221</v>
+      </c>
+      <c r="D55" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" t="s">
+        <v>221</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" t="s">
+        <v>221</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
+        <v>221</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" t="s">
+        <v>221</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="s">
+        <v>221</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" t="s">
+        <v>221</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" t="s">
+        <v>221</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" t="s">
+        <v>221</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="s">
+        <v>221</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" t="s">
+        <v>221</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" t="s">
+        <v>221</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" t="s">
+        <v>221</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="s">
+        <v>221</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C75" t="s">
+        <v>221</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" t="s">
+        <v>221</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>221</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" t="s">
+        <v>221</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" t="s">
+        <v>221</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" t="s">
+        <v>221</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" t="s">
+        <v>221</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" t="s">
+        <v>221</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" t="s">
+        <v>221</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" t="s">
+        <v>221</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C90" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" t="s">
+        <v>221</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" t="s">
+        <v>221</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C93" t="s">
+        <v>221</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" t="s">
+        <v>221</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" t="s">
+        <v>221</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C96" t="s">
+        <v>221</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C97" t="s">
+        <v>221</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" t="s">
+        <v>221</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C99" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C100" t="s">
+        <v>221</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C101" t="s">
+        <v>221</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" t="s">
+        <v>221</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C103" t="s">
+        <v>221</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" t="s">
+        <v>221</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C105" t="s">
+        <v>221</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" t="s">
+        <v>221</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://pfam.xfam.org/family/PF13296" xr:uid="{76FD9689-ABF8-E240-954D-2DE7BA550EEA}"/>
+    <hyperlink ref="B20" r:id="rId2" display="https://pfam.xfam.org/family/PF06812" xr:uid="{9E228770-E181-C84C-9675-02FDBDAED705}"/>
+    <hyperlink ref="B34" r:id="rId3" display="https://pfam.xfam.org/family/PF17541" xr:uid="{19ADF332-CC3A-0043-B2D5-F4EB86E5DE40}"/>
+    <hyperlink ref="D34" r:id="rId4" display="https://pfam.xfam.org/family/PF17541" xr:uid="{F38220E0-FB11-0442-9DFC-3E852865A5F1}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating t6ss.xlsx and Appendix Table S1
</commit_message>
<xml_diff>
--- a/data/t6ss.xlsx
+++ b/data/t6ss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\_home_leep_rfsouza\git\10ksgt6ss\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B74DF4E-CE11-4B57-AE5D-8DEA3D18051F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07E495-9314-4F78-9FDC-8D30D1E87969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{292630A4-619B-0545-B543-097A253988D1}"/>
   </bookViews>
   <sheets>
     <sheet name="t6ss" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="222">
   <si>
     <t>Accession</t>
   </si>
@@ -767,7 +767,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -799,12 +799,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,6 +854,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1152,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E649C-559B-754A-9F35-CCF19D3C1FE3}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
@@ -2006,9 +2032,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90900223-5810-9042-B674-407BA3CF946F}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2016,9 +2044,11 @@
     <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>100</v>
       </c>
@@ -2031,8 +2061,10 @@
       <c r="D1" s="11" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="17"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2046,7 +2078,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -2060,7 +2092,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -2074,7 +2106,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2086,7 +2118,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -2100,7 +2132,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2114,7 +2146,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -2128,7 +2160,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -2142,7 +2174,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -2156,7 +2188,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -2170,7 +2202,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2184,12 +2216,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>101</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>150</v>
@@ -2198,12 +2230,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>150</v>
@@ -2212,12 +2244,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>150</v>
@@ -2226,12 +2258,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>150</v>
@@ -2245,10 +2277,10 @@
         <v>101</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>138</v>
@@ -2259,7 +2291,7 @@
         <v>101</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>156</v>
@@ -2273,7 +2305,7 @@
         <v>101</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>156</v>
@@ -2287,7 +2319,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>156</v>
@@ -2301,7 +2333,7 @@
         <v>101</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>156</v>
@@ -2315,7 +2347,7 @@
         <v>101</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>156</v>
@@ -2329,7 +2361,7 @@
         <v>101</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>156</v>
@@ -2385,13 +2417,11 @@
         <v>101</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>156</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,13 +2429,11 @@
         <v>101</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>156</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2425,7 +2453,7 @@
         <v>101</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
@@ -2437,7 +2465,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
@@ -2449,7 +2477,7 @@
         <v>101</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
@@ -2461,7 +2489,7 @@
         <v>101</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
@@ -2473,7 +2501,7 @@
         <v>101</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
@@ -2485,7 +2513,7 @@
         <v>101</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
@@ -2497,7 +2525,7 @@
         <v>101</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
@@ -2509,7 +2537,7 @@
         <v>101</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
@@ -2521,7 +2549,7 @@
         <v>101</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
@@ -2533,7 +2561,7 @@
         <v>101</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
@@ -2545,7 +2573,7 @@
         <v>101</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
@@ -2557,7 +2585,7 @@
         <v>101</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
@@ -2569,7 +2597,7 @@
         <v>101</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
@@ -2581,7 +2609,7 @@
         <v>101</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
@@ -2617,7 +2645,7 @@
         <v>101</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
@@ -2629,7 +2657,7 @@
         <v>101</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
@@ -2641,7 +2669,7 @@
         <v>101</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
@@ -2653,62 +2681,17 @@
         <v>101</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F49">
+    <sortCondition ref="F2:F49"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>